<commit_message>
Guardar Excel en Datagridview
</commit_message>
<xml_diff>
--- a/proyectos_basic/escritorio/ejemplo.xlsx
+++ b/proyectos_basic/escritorio/ejemplo.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>A</t>
   </si>
@@ -23,6 +24,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -373,15 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,8 +398,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -402,8 +412,11 @@
       <c r="C2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -413,8 +426,11 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -424,8 +440,11 @@
       <c r="C4">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -435,12 +454,70 @@
       <c r="C5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>